<commit_message>
update ingest data process and document
</commit_message>
<xml_diff>
--- a/Azure DW Plan/Dimensional_Modeling_Workbook.xlsx
+++ b/Azure DW Plan/Dimensional_Modeling_Workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8cfe510edd1945de/dev/Training/Git/Self_study/github/training-datawarehouse-restaurant-inspection/Azure DW Plan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{EBB152FD-7891-4964-8573-A27CC82DC39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAC7E8FA-B0D3-4538-9CFE-F29CA39C6070}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{EBB152FD-7891-4964-8573-A27CC82DC39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55E1479A-1225-41C5-8ABB-6C5AE2E9B645}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset Info" sheetId="7" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="271">
   <si>
     <t>Date</t>
   </si>
@@ -1047,10 +1047,17 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1426,304 +1433,307 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="4" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1874,10 +1884,14 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1915,9 +1929,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1950,26 +1964,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2002,26 +1999,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2200,7 +2180,7 @@
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="B12" sqref="B12:B13"/>
     </sheetView>
   </sheetViews>
@@ -2287,7 +2267,7 @@
       <c r="A12" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="101" t="s">
+      <c r="B12" s="85" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2295,7 +2275,7 @@
       <c r="A13" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="102"/>
+      <c r="B13" s="86"/>
     </row>
     <row r="17" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
@@ -2309,7 +2289,7 @@
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="B12:B13"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>frequency</formula1>
@@ -2350,45 +2330,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="93" t="s">
+      <c r="B1" s="95" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="93" t="s">
+      <c r="C1" s="95" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="93" t="s">
+      <c r="D1" s="95" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="93" t="s">
+      <c r="E1" s="95" t="s">
         <v>124</v>
       </c>
-      <c r="F1" s="93" t="s">
+      <c r="F1" s="95" t="s">
         <v>125</v>
       </c>
-      <c r="G1" s="93" t="s">
+      <c r="G1" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="95" t="s">
+      <c r="H1" s="97" t="s">
         <v>120</v>
       </c>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
-      <c r="N1" s="97"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="99"/>
     </row>
     <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="94"/>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
+      <c r="A2" s="96"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
       <c r="H2" s="64" t="s">
         <v>126</v>
       </c>
@@ -2551,45 +2531,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="93" t="s">
+      <c r="B1" s="95" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="93" t="s">
+      <c r="C1" s="95" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="93" t="s">
+      <c r="D1" s="95" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="93" t="s">
+      <c r="E1" s="95" t="s">
         <v>124</v>
       </c>
-      <c r="F1" s="93" t="s">
+      <c r="F1" s="95" t="s">
         <v>125</v>
       </c>
-      <c r="G1" s="93" t="s">
+      <c r="G1" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="95" t="s">
+      <c r="H1" s="97" t="s">
         <v>120</v>
       </c>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
-      <c r="N1" s="97"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="99"/>
     </row>
     <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="94"/>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
+      <c r="A2" s="96"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
       <c r="H2" s="64" t="s">
         <v>126</v>
       </c>
@@ -2753,45 +2733,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="93" t="s">
+      <c r="B1" s="95" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="93" t="s">
+      <c r="C1" s="95" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="93" t="s">
+      <c r="D1" s="95" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="93" t="s">
+      <c r="E1" s="95" t="s">
         <v>124</v>
       </c>
-      <c r="F1" s="93" t="s">
+      <c r="F1" s="95" t="s">
         <v>125</v>
       </c>
-      <c r="G1" s="93" t="s">
+      <c r="G1" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="95" t="s">
+      <c r="H1" s="97" t="s">
         <v>120</v>
       </c>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
-      <c r="N1" s="97"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="99"/>
     </row>
     <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="94"/>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
+      <c r="A2" s="96"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
       <c r="H2" s="64" t="s">
         <v>126</v>
       </c>
@@ -2954,37 +2934,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="98" t="s">
+      <c r="B1" s="100" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="98" t="s">
+      <c r="C1" s="100" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="98" t="s">
+      <c r="D1" s="100" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="98" t="s">
+      <c r="E1" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="95" t="s">
+      <c r="F1" s="97" t="s">
         <v>120</v>
       </c>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="97"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="99"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="99"/>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
+      <c r="A2" s="101"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
       <c r="F2" s="75" t="s">
         <v>126</v>
       </c>
@@ -3245,37 +3225,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="98" t="s">
+      <c r="B1" s="100" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="98" t="s">
+      <c r="C1" s="100" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="98" t="s">
+      <c r="D1" s="100" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="98" t="s">
+      <c r="E1" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="95" t="s">
+      <c r="F1" s="97" t="s">
         <v>120</v>
       </c>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="97"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="99"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="99"/>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
+      <c r="A2" s="101"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
       <c r="F2" s="75" t="s">
         <v>126</v>
       </c>
@@ -3747,10 +3727,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="100"/>
+      <c r="B1" s="102"/>
     </row>
     <row r="2" spans="1:2" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="83" t="s">
@@ -3884,7 +3864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -3898,12 +3878,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="87"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="89"/>
     </row>
     <row r="2" spans="1:4" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
@@ -4144,7 +4124,7 @@
   <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4156,12 +4136,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="7" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="90"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="92"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -4267,7 +4247,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -4281,8 +4261,8 @@
   </sheetPr>
   <dimension ref="C5:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5:J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4301,25 +4281,25 @@
       <c r="C5" s="55" t="s">
         <v>117</v>
       </c>
-      <c r="D5" s="91" t="s">
+      <c r="D5" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="91" t="s">
+      <c r="E5" s="93" t="s">
         <v>104</v>
       </c>
-      <c r="F5" s="91" t="s">
+      <c r="F5" s="93" t="s">
         <v>105</v>
       </c>
-      <c r="G5" s="91" t="s">
+      <c r="G5" s="93" t="s">
         <v>107</v>
       </c>
-      <c r="H5" s="91" t="s">
+      <c r="H5" s="93" t="s">
         <v>106</v>
       </c>
-      <c r="I5" s="91" t="s">
+      <c r="I5" s="93" t="s">
         <v>211</v>
       </c>
-      <c r="J5" s="91" t="s">
+      <c r="J5" s="93" t="s">
         <v>108</v>
       </c>
     </row>
@@ -4327,13 +4307,13 @@
       <c r="C6" s="55" t="s">
         <v>118</v>
       </c>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
-      <c r="F6" s="92"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="92"/>
+      <c r="D6" s="94"/>
+      <c r="E6" s="94"/>
+      <c r="F6" s="94"/>
+      <c r="G6" s="94"/>
+      <c r="H6" s="94"/>
+      <c r="I6" s="94"/>
+      <c r="J6" s="94"/>
     </row>
     <row r="7" spans="3:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="56" t="s">
@@ -4385,7 +4365,7 @@
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="H5:H6"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4401,7 +4381,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomRight" activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4494,7 +4474,7 @@
       <c r="D3" s="48" t="s">
         <v>114</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="103" t="s">
         <v>116</v>
       </c>
       <c r="F3" s="49" t="s">
@@ -4559,8 +4539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39FE541F-35AD-4617-B4E0-3A8EDADA3B2B}">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4580,45 +4560,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="93" t="s">
+      <c r="B1" s="95" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="93" t="s">
+      <c r="C1" s="95" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="93" t="s">
+      <c r="D1" s="95" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="93" t="s">
+      <c r="E1" s="95" t="s">
         <v>124</v>
       </c>
-      <c r="F1" s="93" t="s">
+      <c r="F1" s="95" t="s">
         <v>125</v>
       </c>
-      <c r="G1" s="93" t="s">
+      <c r="G1" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="95" t="s">
+      <c r="H1" s="97" t="s">
         <v>120</v>
       </c>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
-      <c r="N1" s="97"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="99"/>
     </row>
     <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="94"/>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
+      <c r="A2" s="96"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
       <c r="H2" s="64" t="s">
         <v>126</v>
       </c>
@@ -4657,8 +4637,8 @@
       <c r="E3" s="62" t="s">
         <v>134</v>
       </c>
-      <c r="F3" s="62" t="s">
-        <v>135</v>
+      <c r="F3" s="62">
+        <v>2</v>
       </c>
       <c r="G3" s="62"/>
       <c r="H3" s="58" t="s">
@@ -4673,7 +4653,9 @@
       <c r="M3" s="58" t="s">
         <v>138</v>
       </c>
-      <c r="N3" s="58"/>
+      <c r="N3" s="58">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="61" t="s">
@@ -4691,8 +4673,8 @@
       <c r="E4" s="62">
         <v>41669959</v>
       </c>
-      <c r="F4" s="62" t="s">
-        <v>135</v>
+      <c r="F4" s="62">
+        <v>2</v>
       </c>
       <c r="G4" s="62"/>
       <c r="H4" s="58" t="s">
@@ -4791,8 +4773,8 @@
       <c r="E7" s="63">
         <v>45083</v>
       </c>
-      <c r="F7" s="62" t="s">
-        <v>142</v>
+      <c r="F7" s="62">
+        <v>2</v>
       </c>
       <c r="G7" s="62"/>
       <c r="H7" s="58" t="s">
@@ -4823,8 +4805,8 @@
       <c r="E8" s="63">
         <v>2958101</v>
       </c>
-      <c r="F8" s="62" t="s">
-        <v>142</v>
+      <c r="F8" s="62">
+        <v>2</v>
       </c>
       <c r="G8" s="62"/>
       <c r="H8" s="58" t="s">
@@ -4857,8 +4839,8 @@
       <c r="E9" s="62">
         <v>1</v>
       </c>
-      <c r="F9" s="62" t="s">
-        <v>142</v>
+      <c r="F9" s="62">
+        <v>2</v>
       </c>
       <c r="G9" s="62"/>
       <c r="H9" s="58" t="s">
@@ -4915,45 +4897,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="93" t="s">
+      <c r="B1" s="95" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="93" t="s">
+      <c r="C1" s="95" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="93" t="s">
+      <c r="D1" s="95" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="93" t="s">
+      <c r="E1" s="95" t="s">
         <v>124</v>
       </c>
-      <c r="F1" s="93" t="s">
+      <c r="F1" s="95" t="s">
         <v>125</v>
       </c>
-      <c r="G1" s="93" t="s">
+      <c r="G1" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="95" t="s">
+      <c r="H1" s="97" t="s">
         <v>120</v>
       </c>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
-      <c r="N1" s="97"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="99"/>
     </row>
     <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="94"/>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
+      <c r="A2" s="96"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
       <c r="H2" s="64" t="s">
         <v>126</v>
       </c>
@@ -5149,45 +5131,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="93" t="s">
+      <c r="B1" s="95" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="93" t="s">
+      <c r="C1" s="95" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="93" t="s">
+      <c r="D1" s="95" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="93" t="s">
+      <c r="E1" s="95" t="s">
         <v>124</v>
       </c>
-      <c r="F1" s="93" t="s">
+      <c r="F1" s="95" t="s">
         <v>125</v>
       </c>
-      <c r="G1" s="93" t="s">
+      <c r="G1" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="95" t="s">
+      <c r="H1" s="97" t="s">
         <v>120</v>
       </c>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
-      <c r="N1" s="97"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="99"/>
     </row>
     <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="94"/>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
+      <c r="A2" s="96"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
       <c r="H2" s="64" t="s">
         <v>126</v>
       </c>
@@ -5544,45 +5526,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="93" t="s">
+      <c r="B1" s="95" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="93" t="s">
+      <c r="C1" s="95" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="93" t="s">
+      <c r="D1" s="95" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="93" t="s">
+      <c r="E1" s="95" t="s">
         <v>124</v>
       </c>
-      <c r="F1" s="93" t="s">
+      <c r="F1" s="95" t="s">
         <v>125</v>
       </c>
-      <c r="G1" s="93" t="s">
+      <c r="G1" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="95" t="s">
+      <c r="H1" s="97" t="s">
         <v>120</v>
       </c>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
-      <c r="N1" s="97"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="99"/>
     </row>
     <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="94"/>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
+      <c r="A2" s="96"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
       <c r="H2" s="64" t="s">
         <v>126</v>
       </c>

</xml_diff>